<commit_message>
Pushing what i have so far
</commit_message>
<xml_diff>
--- a/Documents/CDR/APG_SrDesCombinedSheet.xlsx
+++ b/Documents/CDR/APG_SrDesCombinedSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\party\ECE590_SeniorDesign\Documents\CDR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMa\Documents\ECE590_SeniorDesign\Documents\CDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F86F53C2-DAD9-402F-ADFB-849D87A78910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED96D3-ACCC-4314-837D-52C9929A9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="2" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Decision Matrix" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>ID</t>
   </si>
@@ -61,9 +62,6 @@
     <t>Concept 3</t>
   </si>
   <si>
-    <t>aalaksnaflkansflkndflkan and a a a a poggers</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -85,16 +83,76 @@
     <t>X</t>
   </si>
   <si>
-    <t>do the thin</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>Weight (1-10)</t>
   </si>
   <si>
     <t>Base line</t>
+  </si>
+  <si>
+    <t>Lightweight</t>
+  </si>
+  <si>
+    <t>Lower Power Consumption</t>
+  </si>
+  <si>
+    <t>Data storage</t>
+  </si>
+  <si>
+    <t>Ease of use</t>
+  </si>
+  <si>
+    <t>Connectivity</t>
+  </si>
+  <si>
+    <t>Reliability</t>
+  </si>
+  <si>
+    <t>Compact</t>
+  </si>
+  <si>
+    <t>Weight &lt; 100 grams</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t>Affordability</t>
+  </si>
+  <si>
+    <t>Produced consitent and reliable data</t>
+  </si>
+  <si>
+    <t>Output Voltage and Current</t>
+  </si>
+  <si>
+    <t>Size: Maxiumum 3 in width, 4 in length</t>
+  </si>
+  <si>
+    <t>Minimize Power Use</t>
+  </si>
+  <si>
+    <t>Desgin Goal: The longer we can power the board the better. Minimum of 2  hours of battery life. Would like 3-4 hours</t>
+  </si>
+  <si>
+    <t>Maximum 200 grams</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Maximum 3 in width, 4 in length</t>
+  </si>
+  <si>
+    <t>$200 or less</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Unit production cost &lt; $200</t>
+  </si>
+  <si>
+    <t>3 inches width, 4 inches length</t>
   </si>
 </sst>
 </file>
@@ -102,7 +160,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -139,23 +197,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -163,6 +218,49 @@
   </cellStyles>
   <dxfs count="28">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -175,79 +273,36 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -263,43 +318,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="20" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:C20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1970D74B-016F-4A7B-BFC2-CE48B6802A0F}" name="ID" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{79D67B5B-C7DD-4F5D-A620-71D3D472C428}" name="Requirement" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{E8B8AFB5-EC8F-492C-B85A-E181CBCAED28}" name="Description" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{1970D74B-016F-4A7B-BFC2-CE48B6802A0F}" name="ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{79D67B5B-C7DD-4F5D-A620-71D3D472C428}" name="Requirement" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{E8B8AFB5-EC8F-492C-B85A-E181CBCAED28}" name="Description" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F20" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F20" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:F20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4067544A-B5B1-407C-BCB1-8EFB196E6CBA}" name="ID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{37A75443-5B97-4524-9648-5A2EE1292343}" name="Requirement" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{F0C64C5C-4182-4645-A6A4-48E3C03C9CDB}" name="Analysis" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{DCA8A0C5-79D1-4FE5-9E99-8B928833FA5F}" name="Demonstration" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{4F9178D9-CFD0-4B00-84D8-C70609794A34}" name="Inspection" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{FAFA5E6F-D494-4A3E-99BA-A83F8B9C4FAA}" name="Test" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{4067544A-B5B1-407C-BCB1-8EFB196E6CBA}" name="ID" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{37A75443-5B97-4524-9648-5A2EE1292343}" name="Requirement" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F0C64C5C-4182-4645-A6A4-48E3C03C9CDB}" name="Analysis" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{DCA8A0C5-79D1-4FE5-9E99-8B928833FA5F}" name="Demonstration" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{4F9178D9-CFD0-4B00-84D8-C70609794A34}" name="Inspection" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FAFA5E6F-D494-4A3E-99BA-A83F8B9C4FAA}" name="Test" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:G20" headerRowDxfId="23" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:G20" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:G20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="27" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="26" totalsRowDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="25" totalsRowDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="17" totalsRowDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="16" totalsRowDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{F3DD4EB5-715A-42E5-BA78-E79DBC5A89A7}" name="Concept 3" totalsRowFunction="count" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{F3DD4EB5-715A-42E5-BA78-E79DBC5A89A7}" name="Concept 3" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -625,13 +680,13 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -640,7 +695,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -650,36 +705,54 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -811,19 +884,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -832,7 +905,7 @@
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -845,7 +918,7 @@
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -858,7 +931,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -871,7 +944,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -882,7 +955,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="4"/>
     </row>
@@ -893,7 +966,7 @@
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -904,7 +977,7 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1045,7 +1118,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,10 +1139,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -1082,11 +1155,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>15</v>
+      <c r="A2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1104,15 +1177,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -1128,8 +1201,12 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C4" s="2">
         <v>1</v>
       </c>
@@ -1145,10 +1222,14 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1160,8 +1241,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="C6" s="2">
         <v>1</v>
       </c>
@@ -1171,8 +1256,12 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="C7" s="2">
         <v>1</v>
       </c>
@@ -1182,8 +1271,12 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
@@ -1193,8 +1286,12 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
@@ -1229,11 +1326,9 @@
       <c r="A12" s="3"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -1317,25 +1412,25 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
         <f>SUMPRODUCT(D2:D19, C2:C19)</f>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2">
         <f>SUMPRODUCT(E2:E19, C2:C19)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F20" s="2">
         <f>SUMPRODUCT(F2:F19, C2:C19)</f>
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G20" s="2">
         <f>SUMPRODUCT(G2:G19, C2:C19)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1349,6 +1444,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ADC84C2C2689F418E5BAD3CA70F51C1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dfa36a507fa972b0dae0ef5557aeb3eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xmlns:ns4="703aeb73-56ce-48f3-9277-f60cff690132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb78c5b39430d5080de0e1d97c12cd45" ns3:_="" ns4:_="">
     <xsd:import namespace="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
@@ -1581,24 +1693,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058E2AD2-D07E-4687-89F2-B97F3F60D89A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1615,29 +1735,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final edits before meeting tomorrow
</commit_message>
<xml_diff>
--- a/Documents/CDR/APG_SrDesCombinedSheet.xlsx
+++ b/Documents/CDR/APG_SrDesCombinedSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMa\Documents\ECE590_SeniorDesign\Documents\CDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BED96D3-ACCC-4314-837D-52C9929A9D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D5488A-7C39-45FE-822B-B64D91E422C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="2" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="1" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Decision Matrix" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -119,9 +118,6 @@
     <t>Affordability</t>
   </si>
   <si>
-    <t>Produced consitent and reliable data</t>
-  </si>
-  <si>
     <t>Output Voltage and Current</t>
   </si>
   <si>
@@ -153,6 +149,33 @@
   </si>
   <si>
     <t>3 inches width, 4 inches length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accuracy </t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Produces data consistantly</t>
+  </si>
+  <si>
+    <t>Produces accurate data</t>
+  </si>
+  <si>
+    <t>Easy to use interface</t>
+  </si>
+  <si>
+    <t>Can store multiple flights worth of data</t>
+  </si>
+  <si>
+    <t>Is effcient with the power it uses.</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Minimize Power Usage</t>
   </si>
 </sst>
 </file>
@@ -680,7 +703,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -706,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -715,10 +738,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -726,10 +749,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -737,10 +760,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -748,10 +771,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -865,8 +888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CF240B-AAE9-4FEE-B42C-6A18977159EA}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,61 +926,71 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
@@ -965,9 +998,7 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
@@ -976,9 +1007,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -1117,8 +1146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263DCEA5-C3BB-4913-9EDE-0D506D5586C3}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1200,12 +1229,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -1226,7 +1255,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1245,7 +1274,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1275,7 +1304,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1290,7 +1319,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1301,8 +1330,12 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="C10" s="2">
         <v>1</v>
       </c>
@@ -1312,8 +1345,12 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
@@ -1453,14 +1490,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ADC84C2C2689F418E5BAD3CA70F51C1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dfa36a507fa972b0dae0ef5557aeb3eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xmlns:ns4="703aeb73-56ce-48f3-9277-f60cff690132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb78c5b39430d5080de0e1d97c12cd45" ns3:_="" ns4:_="">
     <xsd:import namespace="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
@@ -1693,6 +1722,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
   <ds:schemaRefs>
@@ -1702,23 +1739,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058E2AD2-D07E-4687-89F2-B97F3F60D89A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1735,4 +1755,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added 3 things to da excel sheet
</commit_message>
<xml_diff>
--- a/Documents/CDR/APG_SrDesCombinedSheet.xlsx
+++ b/Documents/CDR/APG_SrDesCombinedSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMa\Documents\ECE590_SeniorDesign\Documents\CDR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\party\ECE590_SeniorDesign\Documents\CDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D5488A-7C39-45FE-822B-B64D91E422C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AB4AD2-4D29-4C75-81B8-1B77ED5C36DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="1" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Concept 2</t>
   </si>
   <si>
-    <t>Concept 3</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Weight &lt; 100 grams</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
     <t>Affordability</t>
   </si>
   <si>
@@ -176,6 +170,36 @@
   </si>
   <si>
     <t>Minimize Power Usage</t>
+  </si>
+  <si>
+    <t>Data Logging</t>
+  </si>
+  <si>
+    <t>2S LiPo</t>
+  </si>
+  <si>
+    <t>1.a</t>
+  </si>
+  <si>
+    <t>Data Processing</t>
+  </si>
+  <si>
+    <t>Data Export</t>
+  </si>
+  <si>
+    <t>5.a</t>
+  </si>
+  <si>
+    <t>5.b</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>Minimum 2 hours battery life</t>
+  </si>
+  <si>
+    <t>we good honestly</t>
   </si>
 </sst>
 </file>
@@ -341,8 +365,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:C20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A1:C23" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{1970D74B-016F-4A7B-BFC2-CE48B6802A0F}" name="ID" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{79D67B5B-C7DD-4F5D-A620-71D3D472C428}" name="Requirement" dataDxfId="24"/>
@@ -353,8 +377,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F20" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:F20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F23" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="A1:F23" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{4067544A-B5B1-407C-BCB1-8EFB196E6CBA}" name="ID" dataDxfId="20"/>
     <tableColumn id="2" xr3:uid="{37A75443-5B97-4524-9648-5A2EE1292343}" name="Requirement" dataDxfId="19"/>
@@ -377,7 +401,7 @@
     <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="6"/>
     <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F3DD4EB5-715A-42E5-BA78-E79DBC5A89A7}" name="Concept 3" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{F3DD4EB5-715A-42E5-BA78-E79DBC5A89A7}" name="delete" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -700,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD600D6-464D-4764-A6A7-2CE34AE9ACAC}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -729,151 +753,180 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="C3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -886,10 +939,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CF240B-AAE9-4FEE-B42C-6A18977159EA}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -907,19 +960,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -927,52 +980,52 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
-        <v>2</v>
+      <c r="A3" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -980,43 +1033,51 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2"/>
+      <c r="A8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2"/>
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1024,7 +1085,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="4"/>
@@ -1034,7 +1095,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="4"/>
@@ -1044,7 +1105,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="4"/>
@@ -1054,7 +1115,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
@@ -1064,7 +1125,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
@@ -1074,7 +1135,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
@@ -1084,7 +1145,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
@@ -1094,7 +1155,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
@@ -1104,7 +1165,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="4"/>
@@ -1114,7 +1175,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
@@ -1124,13 +1185,43 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>19</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1147,7 +1238,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,10 +1259,10 @@
         <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
@@ -1180,15 +1271,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1208,10 +1299,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -1231,10 +1322,10 @@
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -1252,10 +1343,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -1271,10 +1362,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -1286,10 +1377,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1301,10 +1392,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -1316,10 +1407,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
@@ -1331,10 +1422,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2">
         <v>1</v>
@@ -1346,10 +1437,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
@@ -1449,7 +1540,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1490,6 +1581,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ADC84C2C2689F418E5BAD3CA70F51C1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dfa36a507fa972b0dae0ef5557aeb3eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xmlns:ns4="703aeb73-56ce-48f3-9277-f60cff690132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb78c5b39430d5080de0e1d97c12cd45" ns3:_="" ns4:_="">
     <xsd:import namespace="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
@@ -1722,14 +1821,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
   <ds:schemaRefs>
@@ -1739,6 +1830,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058E2AD2-D07E-4687-89F2-B97F3F60D89A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1755,21 +1863,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
CDR Tables done yay
</commit_message>
<xml_diff>
--- a/Documents/CDR/APG_SrDesCombinedSheet.xlsx
+++ b/Documents/CDR/APG_SrDesCombinedSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\party\ECE590_SeniorDesign\Documents\CDR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMa\Documents\ECE590_SeniorDesign\Documents\CDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AB4AD2-4D29-4C75-81B8-1B77ED5C36DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB335F73-3CFD-4A74-BC4E-BEA128F0ED13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="1" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>ID</t>
   </si>
@@ -112,21 +112,12 @@
     <t>Affordability</t>
   </si>
   <si>
-    <t>Output Voltage and Current</t>
-  </si>
-  <si>
-    <t>Size: Maxiumum 3 in width, 4 in length</t>
-  </si>
-  <si>
     <t>Minimize Power Use</t>
   </si>
   <si>
     <t>Desgin Goal: The longer we can power the board the better. Minimum of 2  hours of battery life. Would like 3-4 hours</t>
   </si>
   <si>
-    <t>Maximum 200 grams</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -193,13 +184,25 @@
     <t>5.b</t>
   </si>
   <si>
-    <t>delete</t>
-  </si>
-  <si>
     <t>Minimum 2 hours battery life</t>
   </si>
   <si>
-    <t>we good honestly</t>
+    <t xml:space="preserve">Store at least three flights worth of data </t>
+  </si>
+  <si>
+    <t>Be able to process data from sensors into readable flight data</t>
+  </si>
+  <si>
+    <t>Be able to export that data over serial or visualize over WiFi</t>
+  </si>
+  <si>
+    <t>Input Voltage and Current</t>
+  </si>
+  <si>
+    <t>Maximum 100 grams</t>
+  </si>
+  <si>
+    <t>Be able to output data via serial</t>
   </si>
 </sst>
 </file>
@@ -263,13 +266,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -365,43 +362,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C23" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
-  <autoFilter ref="A1:C23" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}" name="Table1" displayName="Table1" ref="A1:C9" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:C9" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1970D74B-016F-4A7B-BFC2-CE48B6802A0F}" name="ID" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{79D67B5B-C7DD-4F5D-A620-71D3D472C428}" name="Requirement" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{E8B8AFB5-EC8F-492C-B85A-E181CBCAED28}" name="Description" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{1970D74B-016F-4A7B-BFC2-CE48B6802A0F}" name="ID" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{79D67B5B-C7DD-4F5D-A620-71D3D472C428}" name="Requirement" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{E8B8AFB5-EC8F-492C-B85A-E181CBCAED28}" name="Description" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F23" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:F23" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{03896142-E9D7-46F4-94C9-5B524C0B31DF}" name="Table14" displayName="Table14" ref="A1:F9" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:F9" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4067544A-B5B1-407C-BCB1-8EFB196E6CBA}" name="ID" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{37A75443-5B97-4524-9648-5A2EE1292343}" name="Requirement" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{F0C64C5C-4182-4645-A6A4-48E3C03C9CDB}" name="Analysis" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{DCA8A0C5-79D1-4FE5-9E99-8B928833FA5F}" name="Demonstration" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{4F9178D9-CFD0-4B00-84D8-C70609794A34}" name="Inspection" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{FAFA5E6F-D494-4A3E-99BA-A83F8B9C4FAA}" name="Test" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{4067544A-B5B1-407C-BCB1-8EFB196E6CBA}" name="ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{37A75443-5B97-4524-9648-5A2EE1292343}" name="Requirement" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{F0C64C5C-4182-4645-A6A4-48E3C03C9CDB}" name="Analysis" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{DCA8A0C5-79D1-4FE5-9E99-8B928833FA5F}" name="Demonstration" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{4F9178D9-CFD0-4B00-84D8-C70609794A34}" name="Inspection" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{FAFA5E6F-D494-4A3E-99BA-A83F8B9C4FAA}" name="Test" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:G20" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:G20" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F3DD4EB5-715A-42E5-BA78-E79DBC5A89A7}" name="delete" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:F12" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:F12" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -726,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD600D6-464D-4764-A6A7-2CE34AE9ACAC}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -753,21 +749,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -775,21 +771,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -797,10 +793,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -808,27 +804,33 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
@@ -941,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CF240B-AAE9-4FEE-B42C-6A18977159EA}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -980,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -991,10 +993,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
@@ -1008,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1022,13 +1024,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1036,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>12</v>
@@ -1050,7 +1052,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1061,32 +1063,34 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>6</v>
-      </c>
+      <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1094,9 +1098,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>7</v>
-      </c>
+      <c r="A11" s="5"/>
       <c r="B11" s="2"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
@@ -1104,9 +1106,7 @@
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>8</v>
-      </c>
+      <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -1114,9 +1114,7 @@
       <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>9</v>
-      </c>
+      <c r="A13" s="5"/>
       <c r="B13" s="2"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -1124,9 +1122,7 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>10</v>
-      </c>
+      <c r="A14" s="5"/>
       <c r="B14" s="2"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1134,9 +1130,7 @@
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>11</v>
-      </c>
+      <c r="A15" s="5"/>
       <c r="B15" s="2"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
@@ -1144,9 +1138,7 @@
       <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>12</v>
-      </c>
+      <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -1154,9 +1146,7 @@
       <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>13</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -1164,9 +1154,7 @@
       <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>14</v>
-      </c>
+      <c r="A18" s="5"/>
       <c r="B18" s="2"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -1174,9 +1162,7 @@
       <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>15</v>
-      </c>
+      <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
@@ -1184,9 +1170,7 @@
       <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>16</v>
-      </c>
+      <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1194,9 +1178,7 @@
       <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>17</v>
-      </c>
+      <c r="A21" s="5"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1204,9 +1186,7 @@
       <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>18</v>
-      </c>
+      <c r="A22" s="5"/>
       <c r="B22" s="2"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1214,9 +1194,7 @@
       <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>19</v>
-      </c>
+      <c r="A23" s="5"/>
       <c r="B23" s="2"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -1235,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263DCEA5-C3BB-4913-9EDE-0D506D5586C3}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1251,7 +1229,7 @@
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1270,11 +1248,8 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -1282,284 +1257,280 @@
         <v>22</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
       <c r="E4" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9</v>
+      </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2">
-        <v>1</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="2">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="2">
-        <v>1</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C11" s="2">
-        <v>1</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2">
+        <f>SUMPRODUCT(D2:D11, C2:C11)</f>
+        <v>305</v>
+      </c>
+      <c r="E12" s="2">
+        <f>SUMPRODUCT(E2:E11, C2:C11)</f>
+        <v>342</v>
+      </c>
+      <c r="F12" s="2">
+        <f>SUMPRODUCT(F2:F11, C2:C11)</f>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="2">
-        <v>1</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="2">
-        <v>1</v>
-      </c>
+      <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="2">
-        <v>1</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
+      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="2">
-        <v>1</v>
-      </c>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="2">
-        <v>1</v>
-      </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2">
-        <f>SUMPRODUCT(D2:D19, C2:C19)</f>
-        <v>2</v>
-      </c>
-      <c r="E20" s="2">
-        <f>SUMPRODUCT(E2:E19, C2:C19)</f>
-        <v>4</v>
-      </c>
-      <c r="F20" s="2">
-        <f>SUMPRODUCT(F2:F19, C2:C19)</f>
-        <v>6</v>
-      </c>
-      <c r="G20" s="2">
-        <f>SUMPRODUCT(G2:G19, C2:C19)</f>
-        <v>4</v>
-      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1581,14 +1552,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ADC84C2C2689F418E5BAD3CA70F51C1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dfa36a507fa972b0dae0ef5557aeb3eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xmlns:ns4="703aeb73-56ce-48f3-9277-f60cff690132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb78c5b39430d5080de0e1d97c12cd45" ns3:_="" ns4:_="">
     <xsd:import namespace="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
@@ -1821,6 +1784,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
   <ds:schemaRefs>
@@ -1830,23 +1801,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058E2AD2-D07E-4687-89F2-B97F3F60D89A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1863,4 +1817,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
stuff i have done
</commit_message>
<xml_diff>
--- a/Documents/CDR/APG_SrDesCombinedSheet.xlsx
+++ b/Documents/CDR/APG_SrDesCombinedSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TheMa\Documents\ECE590_SeniorDesign\Documents\CDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB335F73-3CFD-4A74-BC4E-BEA128F0ED13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDF80DF-19A7-463F-A358-53DFA648A44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" activeTab="1" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
+    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="11388" xr2:uid="{2CD4689F-3B91-4A9B-BAD5-83620747E251}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -247,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -262,12 +262,18 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -303,9 +309,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -389,15 +392,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:F12" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EFBDC17-495E-424A-B2E7-A9D92F80BC8C}" name="Table13" displayName="Table13" ref="A1:F12" headerRowDxfId="0" dataDxfId="12">
   <autoFilter ref="A1:F12" xr:uid="{AB079AC3-D74B-497B-A23B-EB0CC92C94EA}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{92AF8D31-A4D9-41D9-AE17-2408C78AA72C}" name="Need" totalsRowLabel="Total" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B327862F-56CB-4CFA-A83A-F5BE059A3505}" name="Engineering Requirement" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{E1F8879F-1288-4D42-AED0-DFFE6D031015}" name="Weight (1-10)" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4431059E-B0D6-40E3-A454-9886F08E5A28}" name="Base line" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D7B32861-005B-4E40-9A78-4CEEB3E66814}" name="Concept 1" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{45A9A500-68F0-4961-9004-664738D79BAC}" name="Concept 2" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -722,13 +725,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD600D6-464D-4764-A6A7-2CE34AE9ACAC}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.5546875" customWidth="1"/>
     <col min="3" max="3" width="61.6640625" customWidth="1"/>
   </cols>
@@ -943,8 +946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0CF240B-AAE9-4FEE-B42C-6A18977159EA}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1216,36 +1219,36 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.88671875" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1535,7 +1538,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -1552,6 +1555,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009ADC84C2C2689F418E5BAD3CA70F51C1" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dfa36a507fa972b0dae0ef5557aeb3eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xmlns:ns4="703aeb73-56ce-48f3-9277-f60cff690132" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb78c5b39430d5080de0e1d97c12cd45" ns3:_="" ns4:_="">
     <xsd:import namespace="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
@@ -1784,14 +1795,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="218cae68-0ddc-43bb-9a29-52a0402d6cb9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA2A1C8-352A-4F55-842A-E75E3AA79610}">
   <ds:schemaRefs>
@@ -1801,6 +1804,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{058E2AD2-D07E-4687-89F2-B97F3F60D89A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1817,21 +1837,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04E77F84-165D-4CC7-9F9B-4BEDF4DE9229}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="218cae68-0ddc-43bb-9a29-52a0402d6cb9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="703aeb73-56ce-48f3-9277-f60cff690132"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>